<commit_message>
code improve with functions
</commit_message>
<xml_diff>
--- a/Games.xlsx
+++ b/Games.xlsx
@@ -8,7 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Games" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Games PS4" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Games SWITCH" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -767,4 +768,179 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Game</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>JOGO POKÉMON SWORD NINTENDO SWITCH</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>R$ 369,49</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>JOGO MARIO KART 8 DELUXE NINTENDO SWITCH</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>R$ 325,51</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>JOGO POKÉMON LEGENDS: ARCEUS NINTENDO SWITCH</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>R$ 443,43</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>JOGO SUPER SMASH BROS ULTIMATE NINTENDO SWITCH</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>R$ 369,49</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>JOGO POKÉMON LETS GO EEVEE NINTENDO SWITCH</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>R$ 369,49</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>JOGO NEW SUPER MARIO BROS. U DELUXE NINTENDO SWITCH</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>R$ 369,49</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>JOGO POKÉMON SHINING PEARL NINTENDO SWITCH</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>R$ 369,49</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>JOGO THE LEGEND OF ZELDA: TEARS OF THE KINGDOM NINTENDO SWITCH</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>R$ 325,51</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>JOGO MINECRAFT NINTENDO SWITCH</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>R$ 312,19</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>JOGO ANIMAL CROSSING: NEW HORIZONS</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>R$ 307,91</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>JOGO SUPER MARIO ODYSSEY NINTENDO SWITCH</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>R$ 307,91</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>JOGO MARIO STRIKERS BATTLE LEAGUE NINTENDO SWITCH</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>R$ 263,91</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>